<commit_message>
- Fix export empty reports
- Cleanup templates metadata
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -2,12 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\traccar\templates\export\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11535"/>
   </bookViews>
@@ -26,7 +21,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author>Автор</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">

</xml_diff>

<commit_message>
Fix warning about print scale value
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -2,12 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\traccar\templates\export\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="992"/>
   </bookViews>
@@ -26,7 +21,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author>Автор</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
@@ -867,9 +862,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Pass client timezone to excel template - Templates: adjust timezone, use "https" in links
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -94,9 +94,6 @@
     <t>Period:</t>
   </si>
   <si>
-    <t>${"".format('%1$tY-%1$tm-%1$td %1$tH:%1$tM:%1$tS - %2$tY-%2$tm-%2$td %2$tH:%2$tM:%2$tS', from, to)}</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>Attributes</t>
   </si>
   <si>
-    <t>${event.serverTime}</t>
-  </si>
-  <si>
     <t>${event.type}</t>
   </si>
   <si>
@@ -119,6 +113,12 @@
   </si>
   <si>
     <t>${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
+  </si>
+  <si>
+    <t>${from.toString("YYYY.MM.dd HH:mm:ss")+" - "+to.toString("YYYY.MM.dd HH:mm:ss")}</t>
+  </si>
+  <si>
+    <t>${new("org.joda.time.DateTime", event.serverTime, timezone).toString("YYYY.MM.dd HH:mm:ss")}</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
@@ -835,30 +835,30 @@
     </row>
     <row r="8" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use timezone from preferences for excel reports
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -115,10 +115,10 @@
     <t>${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
   </si>
   <si>
-    <t>${from.toString("YYYY.MM.dd HH:mm:ss")+" - "+to.toString("YYYY.MM.dd HH:mm:ss")}</t>
-  </si>
-  <si>
-    <t>${new("org.joda.time.DateTime", event.serverTime, timezone).toString("YYYY.MM.dd HH:mm:ss")}</t>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", event.serverTime, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
@@ -849,7 +849,7 @@
     </row>
     <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Resave export templates in MS Office
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="template" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -35,11 +34,11 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:area(lastCell="E9")</t>
+          <t>jx:area(lastCell="E9")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,11 +48,11 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="E9" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="E9" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +62,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="device.objects", var="event", lastCell="E9")</t>
+          <t>jx:each(items="device.objects", var="event", lastCell="E9")</t>
         </r>
       </text>
     </comment>
@@ -74,70 +73,68 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t xml:space="preserve">Report type:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Device:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${device.deviceName}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${device.groupName}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geofence Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maintenance Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attributes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${dateTool.format("YYYY-MM-dd HH:mm:ss", event.serverTime, locale, timezone)}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${event.type}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${geofenceNames[event.geofenceId]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${maintenanceNames[event.maintenanceId]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
+    <t>Report type:</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Device:</t>
+  </si>
+  <si>
+    <t>${device.deviceName}</t>
+  </si>
+  <si>
+    <t>Group:</t>
+  </si>
+  <si>
+    <t>${device.groupName}</t>
+  </si>
+  <si>
+    <t>Period:</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Geofence Name</t>
+  </si>
+  <si>
+    <t>Maintenance Name</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", event.serverTime, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>${event.type}</t>
+  </si>
+  <si>
+    <t>${geofenceNames[event.geofenceId]}</t>
+  </si>
+  <si>
+    <t>${maintenanceNames[event.maintenanceId]}</t>
+  </si>
+  <si>
+    <t>${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY\ HH:MM:SS"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,22 +143,7 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF444444"/>
       <name val="Calibri"/>
@@ -176,7 +158,7 @@
       <charset val="204"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -191,7 +173,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -199,7 +181,7 @@
       <charset val="204"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -242,120 +224,82 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="15"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Пояснение" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -414,13 +358,29 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -434,9 +394,9 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -448,7 +408,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -458,9 +418,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -479,9 +445,9 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -493,7 +459,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -503,9 +469,15 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -524,9 +496,9 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -538,7 +510,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffffff"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
@@ -548,45 +520,438 @@
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1030" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+  <a:themeElements>
+    <a:clrScheme name="Стандартная">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Стандартная">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Стандартная">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1396396396396"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.7972972972973"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3018018018018"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.518018018018"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.4189189189189"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.6981981981982"/>
+    <col min="1" max="1" width="20.140625"/>
+    <col min="2" max="2" width="29.85546875"/>
+    <col min="3" max="3" width="37.28515625"/>
+    <col min="4" max="4" width="38.5703125"/>
+    <col min="5" max="5" width="55.42578125"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,14 +962,14 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -615,7 +980,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -626,7 +991,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -637,14 +1002,14 @@
       <c r="D6" s="3"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
@@ -661,7 +1026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
@@ -679,13 +1044,8 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Address in events report (fix #4761)
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -29,13 +29,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:area(lastCell="E9")</t>
+          <t xml:space="preserve">jx:area(lastCell="F9")</t>
         </r>
       </text>
     </comment>
@@ -43,13 +43,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="E9" multisheet="sheetNames")</t>
+          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="F9" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
@@ -57,13 +57,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="11"/>
             <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="device.objects", var="event", lastCell="E9")</t>
+          <t xml:space="preserve">jx:each(items="device.objects", var="event", lastCell="F9")</t>
         </r>
       </text>
     </comment>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Report type:</t>
   </si>
@@ -110,6 +110,9 @@
     <t xml:space="preserve">Maintenance Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attributes</t>
   </si>
   <si>
@@ -123,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">${maintenanceNames[event.maintenanceId]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${positions[event.positionId] != null ? util.hyperlink("".format("https://www.openstreetmap.org/?mlat=%1$f&amp;mlon=%2$f#map=16/%1$f/%2$f", positions[event.positionId].latitude, positions[event.positionId].longitude), positions[event.positionId].getAddress() == null ? "".format("%1$f°, %2$f°", positions[event.positionId].latitude, positions[event.positionId].longitude) : positions[event.positionId].address) : ""}</t>
   </si>
   <si>
     <t xml:space="preserve">${event.attributes.toString().replaceAll(",", " ").replaceAll(bracketsRegex, "")}</t>
@@ -214,11 +220,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -279,44 +285,48 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,15 +334,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,7 +384,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0070C0"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -411,7 +425,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -420,9 +434,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3685680</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:colOff>3685320</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -432,7 +446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12565800" cy="9524520"/>
+          <a:ext cx="12556440" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -456,7 +470,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -465,9 +479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3685680</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:colOff>3685320</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -477,7 +491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12565800" cy="9524520"/>
+          <a:ext cx="12556440" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -501,7 +515,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -510,9 +524,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3685680</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:colOff>3685320</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -522,7 +536,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12565800" cy="9524520"/>
+          <a:ext cx="12556440" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -546,7 +560,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -555,9 +569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -567,7 +581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10013400" cy="9524520"/>
+          <a:ext cx="10004040" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -591,7 +605,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -600,9 +614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -612,7 +626,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10013400" cy="9524520"/>
+          <a:ext cx="10004040" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -636,7 +650,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -645,9 +659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:colOff>1132920</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -657,7 +671,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10013400" cy="9524520"/>
+          <a:ext cx="10004040" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -685,127 +699,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="55.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="A1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>12</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>17</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>